<commit_message>
Added ML for hackers
</commit_message>
<xml_diff>
--- a/Presentation/R.xlsx
+++ b/Presentation/R.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\R4DotNet\Presentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t xml:space="preserve">R </t>
   </si>
@@ -151,13 +156,22 @@
   </si>
   <si>
     <t>Turn continous to catagorical</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +183,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -218,10 +239,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -231,6 +252,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -279,7 +303,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -314,7 +338,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -523,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E33"/>
+  <dimension ref="B2:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,9 +558,8 @@
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" customWidth="1"/>
-    <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
@@ -545,10 +568,10 @@
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -585,150 +608,183 @@
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>36</v>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C29" t="s">
         <v>7</v>
       </c>
-      <c r="E23" t="s">
+      <c r="D29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>23</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C30" t="s">
         <v>15</v>
       </c>
-      <c r="E24" t="s">
+      <c r="D30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>9</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C31" t="s">
         <v>17</v>
       </c>
-      <c r="E25" t="s">
+      <c r="D31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C32" t="s">
         <v>16</v>
       </c>
-      <c r="E26" t="s">
+      <c r="D32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>7</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C33" t="s">
         <v>20</v>
       </c>
-      <c r="E27" t="s">
+      <c r="D33" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>42</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>43</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C39" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Additional changes to the code
</commit_message>
<xml_diff>
--- a/Presentation/R.xlsx
+++ b/Presentation/R.xlsx
@@ -143,12 +143,6 @@
     <t>Use cut</t>
   </si>
   <si>
-    <t>Col/Row* in a spreadsheet</t>
-  </si>
-  <si>
-    <t>Col*/Row in a spreadsheet</t>
-  </si>
-  <si>
     <t>Indepedent varaible</t>
   </si>
   <si>
@@ -165,6 +159,12 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>Col in a spreadsheet</t>
+  </si>
+  <si>
+    <t>Row in a spreadsheet</t>
   </si>
 </sst>
 </file>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,10 +617,10 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
@@ -677,7 +677,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -704,7 +704,7 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -715,7 +715,7 @@
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -737,7 +737,7 @@
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
@@ -774,7 +774,7 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
         <v>26</v>
@@ -782,7 +782,7 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Added more updates for regression
</commit_message>
<xml_diff>
--- a/Presentation/R.xlsx
+++ b/Presentation/R.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\R4DotNet\Presentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="20640" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t xml:space="preserve">R </t>
   </si>
@@ -165,13 +160,16 @@
   </si>
   <si>
     <t>Row in a spreadsheet</t>
+  </si>
+  <si>
+    <t>y = X1 + X2 + X3 + E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,7 +301,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -335,10 +333,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -370,7 +367,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -546,14 +542,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
@@ -562,12 +558,12 @@
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -575,7 +571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -583,7 +579,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -591,7 +587,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -599,7 +595,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -607,7 +603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3">
       <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
@@ -615,7 +611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3">
       <c r="B10" t="s">
         <v>44</v>
       </c>
@@ -623,12 +619,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3">
       <c r="B13" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3">
       <c r="B14" t="s">
         <v>25</v>
       </c>
@@ -636,22 +632,22 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3">
       <c r="C15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3">
       <c r="C16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4">
       <c r="C17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4">
       <c r="B19" t="s">
         <v>28</v>
       </c>
@@ -659,17 +655,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4">
       <c r="C20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4">
       <c r="C21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4">
       <c r="B23" s="2" t="s">
         <v>0</v>
       </c>
@@ -680,7 +676,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4">
       <c r="B24" t="s">
         <v>3</v>
       </c>
@@ -691,12 +687,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4">
       <c r="B27" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4">
       <c r="B28" s="2" t="s">
         <v>0</v>
       </c>
@@ -707,7 +703,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4">
       <c r="B29" s="3" t="s">
         <v>8</v>
       </c>
@@ -718,7 +714,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4">
       <c r="B30" t="s">
         <v>23</v>
       </c>
@@ -729,7 +725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4">
       <c r="B31" t="s">
         <v>9</v>
       </c>
@@ -740,7 +736,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4">
       <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
@@ -751,7 +747,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4">
       <c r="B33" t="s">
         <v>7</v>
       </c>
@@ -762,17 +758,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4">
       <c r="B35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4">
       <c r="B37" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4">
       <c r="B38" t="s">
         <v>40</v>
       </c>
@@ -780,12 +776,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4">
       <c r="B39" t="s">
         <v>41</v>
       </c>
       <c r="C39" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -795,24 +796,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more changes day of :-)
</commit_message>
<xml_diff>
--- a/Presentation/R.xlsx
+++ b/Presentation/R.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\R4DotNet\Presentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="20640" windowHeight="11760"/>
+    <workbookView xWindow="480" yWindow="36" windowWidth="20640" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -138,9 +143,6 @@
     <t>Use cut</t>
   </si>
   <si>
-    <t>Indepedent varaible</t>
-  </si>
-  <si>
     <t>Dependent variable</t>
   </si>
   <si>
@@ -163,13 +165,16 @@
   </si>
   <si>
     <t>y = X1 + X2 + X3 + E</t>
+  </si>
+  <si>
+    <t>Indepedent variable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,7 +306,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,9 +338,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -367,6 +373,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -542,28 +549,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -571,7 +578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -579,7 +586,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -587,7 +594,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -595,7 +602,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -603,7 +610,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
@@ -611,20 +618,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
         <v>44</v>
       </c>
-      <c r="C10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3">
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>25</v>
       </c>
@@ -632,22 +639,22 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>28</v>
       </c>
@@ -655,17 +662,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>0</v>
       </c>
@@ -673,10 +680,10 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>3</v>
       </c>
@@ -687,12 +694,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>0</v>
       </c>
@@ -700,10 +707,10 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>8</v>
       </c>
@@ -711,10 +718,10 @@
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>23</v>
       </c>
@@ -725,7 +732,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>9</v>
       </c>
@@ -733,10 +740,10 @@
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
@@ -747,7 +754,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>7</v>
       </c>
@@ -758,35 +765,35 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="2:4">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -796,24 +803,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>